<commit_message>
feat: Real use-case test implemented
</commit_message>
<xml_diff>
--- a/Protocol/src/ExcelToAppComponent/Eolian_auriga/components.xlsx
+++ b/Protocol/src/ExcelToAppComponent/Eolian_auriga/components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github\Eolian-Telemetria-Auriga\Protocol\src\ExcelToAppComponent\Eolian_auriga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4372DA1-3B40-46C7-8AB5-664854981432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D1117-43D3-4C4C-A836-455D004E9B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inversor_der" sheetId="2" r:id="rId1"/>
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B547D1-632A-4F3B-9A3A-887796921B5F}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D22A6-69A3-4C78-81BF-9DE38D1DB719}">
   <dimension ref="A1:BH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>